<commit_message>
Some changes related with optional column
</commit_message>
<xml_diff>
--- a/test/EPPlus.Core.Extensions.Tests/Resources/testsheets1.xlsx
+++ b/test/EPPlus.Core.Extensions.Tests/Resources/testsheets1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Workspace\EPPlus.Core.Extensions\test\EPPlus.Core.Extensions.Tests\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayer02\Desktop\Desktop\repos\EPPlus.Core.Extensions\test\EPPlus.Core.Extensions.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FF699B-5405-43CF-9364-04716DD6DC8A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="7"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEST1" sheetId="1" r:id="rId1"/>
@@ -21,12 +22,20 @@
     <sheet name="TEST7" sheetId="7" r:id="rId7"/>
     <sheet name="EmptySheet" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -168,11 +177,14 @@
   <si>
     <t>Barcode3</t>
   </si>
+  <si>
+    <t>Optional1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0\ [$USD]"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
@@ -231,7 +243,7 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="167" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -267,52 +279,53 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TEST1" displayName="TEST1" ref="A1:E6" totalsRowShown="0">
-  <autoFilter ref="A1:E6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TEST1" displayName="TEST1" ref="A1:E6" totalsRowShown="0">
+  <autoFilter ref="A1:E6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name"/>
-    <tableColumn id="2" name="Birth Date"/>
-    <tableColumn id="3" name="Gender"/>
-    <tableColumn id="5" name="Class"/>
-    <tableColumn id="4" name="Height"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Birth Date"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Gender"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Class"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Height"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TEST2" displayName="TEST2" ref="A1:B6" totalsRowShown="0">
-  <autoFilter ref="A1:B6"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Car name"/>
-    <tableColumn id="2" name="Price" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TEST2" displayName="TEST2" ref="A1:C6" totalsRowShown="0">
+  <autoFilter ref="A1:C6" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Car name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Price" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{325F2846-1026-45CE-9CCE-27768FE13FD8}" name="Optional1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TEST3" displayName="TEST3" ref="B2:G8" totalsRowCount="1">
-  <autoFilter ref="B2:G7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="TEST3" displayName="TEST3" ref="B2:G8" totalsRowCount="1">
+  <autoFilter ref="B2:G7" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="License plate" totalsRowLabel="Összeg"/>
-    <tableColumn id="2" name="Manufacturer"/>
-    <tableColumn id="3" name="Manufacturing date" totalsRowFunction="max"/>
-    <tableColumn id="4" name="Price" totalsRowFunction="max"/>
-    <tableColumn id="5" name="Color"/>
-    <tableColumn id="6" name="Is ready for traffic?" totalsRowFunction="count"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="License plate" totalsRowLabel="Összeg"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Manufacturer"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Manufacturing date" totalsRowFunction="max"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Price" totalsRowFunction="max"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Color"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Is ready for traffic?" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TEST4" displayName="TEST4" ref="E9:G13" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="E9:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="TEST4" displayName="TEST4" ref="E9:G13" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="E9:G13" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Barcode"/>
-    <tableColumn id="2" name="Quantity"/>
-    <tableColumn id="3" name="UpdatedDate" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Barcode"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Quantity"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="UpdatedDate" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -394,6 +407,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -429,6 +459,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -604,21 +651,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="4" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="4" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -652,7 +699,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -669,7 +716,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -686,7 +733,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -703,7 +750,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -729,28 +776,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -758,7 +808,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -766,19 +816,22 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -796,23 +849,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>29</v>
       </c>
@@ -832,7 +885,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>22</v>
       </c>
@@ -852,7 +905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -872,7 +925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -892,7 +945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>18</v>
       </c>
@@ -909,7 +962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>21</v>
       </c>
@@ -926,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>34</v>
       </c>
@@ -952,20 +1005,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="E9:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E9" s="3" t="s">
         <v>35</v>
       </c>
@@ -976,7 +1029,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
         <v>38</v>
       </c>
@@ -984,7 +1037,7 @@
         <v>42964</v>
       </c>
     </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
         <v>39</v>
       </c>
@@ -995,7 +1048,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
         <v>42</v>
       </c>
@@ -1006,7 +1059,7 @@
         <v>42964.470081018517</v>
       </c>
     </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>43</v>
       </c>
@@ -1024,19 +1077,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
@@ -1047,7 +1100,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1058,7 +1111,7 @@
         <v>42955</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -1069,7 +1122,7 @@
         <v>42955</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1087,19 +1140,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -1113,7 +1166,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1126,7 +1179,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1139,7 +1192,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1153,16 +1206,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
@@ -1179,14 +1232,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Now you can set a column to optional when parsing a sheet, - and incremented version number (v2.4.0)
</commit_message>
<xml_diff>
--- a/test/EPPlus.Core.Extensions.Tests/Resources/testsheets1.xlsx
+++ b/test/EPPlus.Core.Extensions.Tests/Resources/testsheets1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayer02\Desktop\Desktop\repos\EPPlus.Core.Extensions\test\EPPlus.Core.Extensions.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FF699B-5405-43CF-9364-04716DD6DC8A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5087537C-9721-4165-91EA-918241BA456B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEST1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="TEST6" sheetId="6" r:id="rId6"/>
     <sheet name="TEST7" sheetId="7" r:id="rId7"/>
     <sheet name="EmptySheet" sheetId="8" r:id="rId8"/>
+    <sheet name="WithOptionalFields" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -179,6 +180,30 @@
   </si>
   <si>
     <t>Optional1</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Aydin</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Eraydin</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>Age</t>
   </si>
 </sst>
 </file>
@@ -779,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -1243,4 +1268,64 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEED47F8-1EA7-4B69-83CC-0C2A1FFA20B5}">
+  <dimension ref="D4:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="1">
+        <v>43497</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>